<commit_message>
Update supporting material B.xlsx
Correcting error in calculation for one experiment*set for TAN sep eff
</commit_message>
<xml_diff>
--- a/2022_slurry_separation_manuscript/lit_data/supporting material B.xlsx
+++ b/2022_slurry_separation_manuscript/lit_data/supporting material B.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au583430\OneDrive - Aarhus Universitet\Dokumenter\GitHub\slurry-sep-man\lit_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Documents/GitHub/AU-MHB/2022_slurry_separation_manuscript/lit_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B884A39-CF75-409E-BF3B-8837CB992668}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0B884A39-CF75-409E-BF3B-8837CB992668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{400BEB23-2377-42EA-95B8-F14225EE79D1}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1395" windowWidth="21600" windowHeight="9165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31005" yWindow="510" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emission data" sheetId="3" r:id="rId1"/>
     <sheet name="separation efficiency data" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2777,8 +2782,8 @@
   </sheetPr>
   <dimension ref="A1:AL193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15776,11 +15781,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035B63CE-A644-473A-8A37-A055E54316D7}">
   <dimension ref="A1:V251"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F202" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="F235" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G225" sqref="G225"/>
+      <selection pane="bottomRight" activeCell="G254" sqref="G254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19336,8 +19341,8 @@
         <v>71.46817895400126</v>
       </c>
       <c r="G100" s="22">
-        <f>J100*H100/J99</f>
-        <v>71.46817895400126</v>
+        <f>L100*H100/L99</f>
+        <v>90.306905370843992</v>
       </c>
       <c r="H100" s="22">
         <f>(J99-J101)/(J100-J101)*100</f>
@@ -19374,8 +19379,8 @@
         <v>28.531821045998747</v>
       </c>
       <c r="G101" s="22">
-        <f>J101*H101/J99</f>
-        <v>28.531821045998747</v>
+        <f>L101*H101/L99</f>
+        <v>6.7519181585677766</v>
       </c>
       <c r="H101" s="22">
         <f>100-H100</f>
@@ -24510,18 +24515,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24544,14 +24549,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DF2204-8892-4A94-90A5-6DCDBF4AC498}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A402CE-7A4B-44ED-A208-3884D1FBDB29}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -24566,4 +24563,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DF2204-8892-4A94-90A5-6DCDBF4AC498}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
making copy of sep eff data for work in AU-MHB/internal/2024_sep_eff_dig
</commit_message>
<xml_diff>
--- a/2022_slurry_separation_manuscript/lit_data/supporting material B.xlsx
+++ b/2022_slurry_separation_manuscript/lit_data/supporting material B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Documents/GitHub/AU-MHB/2022_slurry_separation_manuscript/lit_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0B884A39-CF75-409E-BF3B-8837CB992668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{400BEB23-2377-42EA-95B8-F14225EE79D1}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{0B884A39-CF75-409E-BF3B-8837CB992668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38C4ACAF-CFFC-48B9-B0B3-75609FF7EE21}"/>
   <bookViews>
-    <workbookView xWindow="-31005" yWindow="510" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31350" yWindow="165" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emission data" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="320">
   <si>
     <t>General information</t>
   </si>
@@ -2063,9 +2063,6 @@
   </si>
   <si>
     <t>Møller et al. (2000)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lf </t>
   </si>
   <si>
     <t>Møller et al. (2002)</t>
@@ -15785,7 +15782,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F235" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G254" sqref="G254"/>
+      <selection pane="bottomRight" activeCell="D249" sqref="D249:D251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19430,7 +19427,7 @@
         <v>61</v>
       </c>
       <c r="D103" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="E103">
         <v>2</v>
@@ -19511,7 +19508,7 @@
         <v>61</v>
       </c>
       <c r="D106" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="E106">
         <v>3</v>
@@ -19592,7 +19589,7 @@
         <v>74</v>
       </c>
       <c r="D109" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="E109">
         <v>7</v>
@@ -19673,7 +19670,7 @@
         <v>74</v>
       </c>
       <c r="D112" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="E112">
         <v>8</v>
@@ -19722,7 +19719,7 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B114" t="s">
         <v>117</v>
@@ -19746,12 +19743,12 @@
         <v>3.6</v>
       </c>
       <c r="M114" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B115" t="s">
         <v>117</v>
@@ -19777,12 +19774,12 @@
         <v>2.77</v>
       </c>
       <c r="M115" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B116" t="s">
         <v>117</v>
@@ -19807,12 +19804,12 @@
         <v>24.56</v>
       </c>
       <c r="M116" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B117" t="s">
         <v>117</v>
@@ -19836,12 +19833,12 @@
         <v>3.5</v>
       </c>
       <c r="M117" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B118" t="s">
         <v>117</v>
@@ -19867,12 +19864,12 @@
         <v>2.84</v>
       </c>
       <c r="M118" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B119" t="s">
         <v>117</v>
@@ -19897,12 +19894,12 @@
         <v>27.93</v>
       </c>
       <c r="M119" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B120" t="s">
         <v>117</v>
@@ -19926,12 +19923,12 @@
         <v>1.3</v>
       </c>
       <c r="M120" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B121" t="s">
         <v>117</v>
@@ -19957,12 +19954,12 @@
         <v>1.39</v>
       </c>
       <c r="M121" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B122" t="s">
         <v>117</v>
@@ -19987,12 +19984,12 @@
         <v>18.73</v>
       </c>
       <c r="M122" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B123" t="s">
         <v>117</v>
@@ -20016,12 +20013,12 @@
         <v>3</v>
       </c>
       <c r="M123" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B124" t="s">
         <v>117</v>
@@ -20047,12 +20044,12 @@
         <v>1.75</v>
       </c>
       <c r="M124" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B125" t="s">
         <v>117</v>
@@ -20077,12 +20074,12 @@
         <v>17.82</v>
       </c>
       <c r="M125" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B126" t="s">
         <v>117</v>
@@ -20106,12 +20103,12 @@
         <v>1.7</v>
       </c>
       <c r="M126" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B127" t="s">
         <v>117</v>
@@ -20137,12 +20134,12 @@
         <v>3.02</v>
       </c>
       <c r="M127" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B128" t="s">
         <v>117</v>
@@ -20167,12 +20164,12 @@
         <v>19.91</v>
       </c>
       <c r="M128" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B129" t="s">
         <v>117</v>
@@ -20196,12 +20193,12 @@
         <v>1.6</v>
       </c>
       <c r="M129" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B130" t="s">
         <v>117</v>
@@ -20227,12 +20224,12 @@
         <v>2.75</v>
       </c>
       <c r="M130" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B131" t="s">
         <v>117</v>
@@ -20257,12 +20254,12 @@
         <v>20.78</v>
       </c>
       <c r="M131" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B132" t="s">
         <v>117</v>
@@ -20286,12 +20283,12 @@
         <v>1.5</v>
       </c>
       <c r="M132" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B133" t="s">
         <v>117</v>
@@ -20317,12 +20314,12 @@
         <v>2.46</v>
       </c>
       <c r="M133" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B134" t="s">
         <v>117</v>
@@ -20347,12 +20344,12 @@
         <v>21.24</v>
       </c>
       <c r="M134" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B135" t="s">
         <v>117</v>
@@ -20376,12 +20373,12 @@
         <v>2.8</v>
       </c>
       <c r="M135" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B136" t="s">
         <v>117</v>
@@ -20407,12 +20404,12 @@
         <v>2.23</v>
       </c>
       <c r="M136" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B137" t="s">
         <v>117</v>
@@ -20437,12 +20434,12 @@
         <v>28.08</v>
       </c>
       <c r="M137" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B138" t="s">
         <v>117</v>
@@ -20466,12 +20463,12 @@
         <v>4</v>
       </c>
       <c r="M138" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B139" t="s">
         <v>117</v>
@@ -20497,12 +20494,12 @@
         <v>2.44</v>
       </c>
       <c r="M139" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B140" t="s">
         <v>117</v>
@@ -20527,12 +20524,12 @@
         <v>25.27</v>
       </c>
       <c r="M140" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B141" t="s">
         <v>117</v>
@@ -20556,12 +20553,12 @@
         <v>3.1</v>
       </c>
       <c r="M141" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B142" t="s">
         <v>117</v>
@@ -20587,12 +20584,12 @@
         <v>1.96</v>
       </c>
       <c r="M142" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B143" t="s">
         <v>117</v>
@@ -20617,12 +20614,12 @@
         <v>29.99</v>
       </c>
       <c r="M143" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B144" t="s">
         <v>117</v>
@@ -20646,12 +20643,12 @@
         <v>2.4</v>
       </c>
       <c r="M144" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B145" t="s">
         <v>117</v>
@@ -20677,12 +20674,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="M145" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B146" t="s">
         <v>117</v>
@@ -20707,12 +20704,12 @@
         <v>20.190000000000001</v>
       </c>
       <c r="M146" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B147" t="s">
         <v>139</v>
@@ -20736,12 +20733,12 @@
         <v>3.6</v>
       </c>
       <c r="M147" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B148" t="s">
         <v>139</v>
@@ -20767,12 +20764,12 @@
         <v>4.25</v>
       </c>
       <c r="M148" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B149" t="s">
         <v>139</v>
@@ -20797,12 +20794,12 @@
         <v>34.44</v>
       </c>
       <c r="M149" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B150" t="s">
         <v>139</v>
@@ -20826,12 +20823,12 @@
         <v>1.7</v>
       </c>
       <c r="M150" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B151" t="s">
         <v>139</v>
@@ -20857,12 +20854,12 @@
         <v>4.63</v>
       </c>
       <c r="M151" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B152" t="s">
         <v>139</v>
@@ -20887,12 +20884,12 @@
         <v>36.47</v>
       </c>
       <c r="M152" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B153" t="s">
         <v>139</v>
@@ -20916,12 +20913,12 @@
         <v>1.5</v>
       </c>
       <c r="M153" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B154" t="s">
         <v>139</v>
@@ -20947,12 +20944,12 @@
         <v>4.03</v>
       </c>
       <c r="M154" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B155" t="s">
         <v>139</v>
@@ -20977,12 +20974,12 @@
         <v>24.97</v>
       </c>
       <c r="M155" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B156" t="s">
         <v>139</v>
@@ -21006,12 +21003,12 @@
         <v>2.8</v>
       </c>
       <c r="M156" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B157" t="s">
         <v>139</v>
@@ -21037,12 +21034,12 @@
         <v>5.23</v>
       </c>
       <c r="M157" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B158" t="s">
         <v>139</v>
@@ -21067,12 +21064,12 @@
         <v>26.84</v>
       </c>
       <c r="M158" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B159" t="s">
         <v>139</v>
@@ -21096,12 +21093,12 @@
         <v>2.4</v>
       </c>
       <c r="M159" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B160" t="s">
         <v>139</v>
@@ -21127,12 +21124,12 @@
         <v>2.95</v>
       </c>
       <c r="M160" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B161" t="s">
         <v>139</v>
@@ -21157,12 +21154,12 @@
         <v>29.84</v>
       </c>
       <c r="M161" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B162" t="s">
         <v>117</v>
@@ -21183,12 +21180,12 @@
         <v>3.9</v>
       </c>
       <c r="M162" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B163" t="s">
         <v>117</v>
@@ -21221,12 +21218,12 @@
         <v>3.8</v>
       </c>
       <c r="M163" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B164" t="s">
         <v>117</v>
@@ -21259,12 +21256,12 @@
         <v>4</v>
       </c>
       <c r="M164" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B165" t="s">
         <v>117</v>
@@ -21285,12 +21282,12 @@
         <v>2.7</v>
       </c>
       <c r="M165" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B166" t="s">
         <v>117</v>
@@ -21323,12 +21320,12 @@
         <v>2.6</v>
       </c>
       <c r="M166" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B167" t="s">
         <v>117</v>
@@ -21361,12 +21358,12 @@
         <v>3.1</v>
       </c>
       <c r="M167" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B168" t="s">
         <v>117</v>
@@ -21387,12 +21384,12 @@
         <v>3.8</v>
       </c>
       <c r="M168" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B169" t="s">
         <v>117</v>
@@ -21425,12 +21422,12 @@
         <v>3.4</v>
       </c>
       <c r="M169" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B170" t="s">
         <v>117</v>
@@ -21463,12 +21460,12 @@
         <v>4.7</v>
       </c>
       <c r="M170" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B171" t="s">
         <v>117</v>
@@ -21489,12 +21486,12 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="M171" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B172" t="s">
         <v>117</v>
@@ -21527,12 +21524,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="M172" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B173" t="s">
         <v>117</v>
@@ -21565,12 +21562,12 @@
         <v>1.7</v>
       </c>
       <c r="M173" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B174" t="s">
         <v>117</v>
@@ -21591,12 +21588,12 @@
         <v>4.62</v>
       </c>
       <c r="M174" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B175" t="s">
         <v>117</v>
@@ -21629,12 +21626,12 @@
         <v>4.5</v>
       </c>
       <c r="M175" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B176" t="s">
         <v>117</v>
@@ -21667,12 +21664,12 @@
         <v>3.3</v>
       </c>
       <c r="M176" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B177" t="s">
         <v>117</v>
@@ -21693,12 +21690,12 @@
         <v>4.62</v>
       </c>
       <c r="M177" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B178" t="s">
         <v>117</v>
@@ -21731,12 +21728,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M178" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B179" t="s">
         <v>117</v>
@@ -21769,12 +21766,12 @@
         <v>3.5</v>
       </c>
       <c r="M179" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B180" t="s">
         <v>117</v>
@@ -21795,12 +21792,12 @@
         <v>4.62</v>
       </c>
       <c r="M180" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B181" t="s">
         <v>117</v>
@@ -21833,12 +21830,12 @@
         <v>4.2</v>
       </c>
       <c r="M181" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B182" t="s">
         <v>117</v>
@@ -21871,12 +21868,12 @@
         <v>4.8</v>
       </c>
       <c r="M182" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B183" t="s">
         <v>117</v>
@@ -21897,12 +21894,12 @@
         <v>4.62</v>
       </c>
       <c r="M183" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B184" t="s">
         <v>117</v>
@@ -21935,12 +21932,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M184" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B185" t="s">
         <v>117</v>
@@ -21973,12 +21970,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M185" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B186" t="s">
         <v>117</v>
@@ -21999,12 +21996,12 @@
         <v>4.62</v>
       </c>
       <c r="M186" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B187" t="s">
         <v>117</v>
@@ -22037,12 +22034,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M187" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B188" t="s">
         <v>117</v>
@@ -22075,12 +22072,12 @@
         <v>3.6</v>
       </c>
       <c r="M188" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B189" t="s">
         <v>117</v>
@@ -22101,12 +22098,12 @@
         <v>4.62</v>
       </c>
       <c r="M189" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B190" t="s">
         <v>117</v>
@@ -22139,12 +22136,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M190" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B191" t="s">
         <v>117</v>
@@ -22177,12 +22174,12 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="M191" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B192" t="s">
         <v>117</v>
@@ -22203,12 +22200,12 @@
         <v>4.62</v>
       </c>
       <c r="M192" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B193" t="s">
         <v>117</v>
@@ -22241,12 +22238,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M193" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B194" t="s">
         <v>117</v>
@@ -22279,12 +22276,12 @@
         <v>3.5</v>
       </c>
       <c r="M194" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B195" t="s">
         <v>117</v>
@@ -22305,12 +22302,12 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="M195" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B196" t="s">
         <v>117</v>
@@ -22343,12 +22340,12 @@
         <v>4.58</v>
       </c>
       <c r="M196" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B197" t="s">
         <v>117</v>
@@ -22381,12 +22378,12 @@
         <v>4.72</v>
       </c>
       <c r="M197" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B198" t="s">
         <v>117</v>
@@ -22407,12 +22404,12 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="M198" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B199" t="s">
         <v>117</v>
@@ -22445,12 +22442,12 @@
         <v>455</v>
       </c>
       <c r="M199" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B200" t="s">
         <v>117</v>
@@ -22483,12 +22480,12 @@
         <v>5.13</v>
       </c>
       <c r="M200" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B201" t="s">
         <v>117</v>
@@ -22509,12 +22506,12 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="M201" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B202" t="s">
         <v>117</v>
@@ -22547,12 +22544,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M202" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B203" t="s">
         <v>117</v>
@@ -22585,12 +22582,12 @@
         <v>4.74</v>
       </c>
       <c r="M203" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B204" t="s">
         <v>139</v>
@@ -22605,7 +22602,7 @@
         <v>14</v>
       </c>
       <c r="I204" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J204" s="21">
         <f>AVERAGE(3.73,3.81)</f>
@@ -22618,7 +22615,7 @@
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B205" t="s">
         <v>139</v>
@@ -22641,19 +22638,19 @@
         <v>91</v>
       </c>
       <c r="I205" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J205" s="24">
         <f>AVERAGE(2.41,2.43,2.59,2.37)</f>
         <v>2.4500000000000002</v>
       </c>
       <c r="M205" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B206" t="s">
         <v>139</v>
@@ -22676,19 +22673,19 @@
         <v>9</v>
       </c>
       <c r="I206" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J206" s="24">
         <f>AVERAGE(22.35,21.8)</f>
         <v>22.075000000000003</v>
       </c>
       <c r="M206" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B207" t="s">
         <v>139</v>
@@ -22703,7 +22700,7 @@
         <v>2</v>
       </c>
       <c r="I207" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J207" s="24">
         <f>AVERAGE(5.74,5.82)</f>
@@ -22720,7 +22717,7 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B208" t="s">
         <v>139</v>
@@ -22729,7 +22726,7 @@
         <v>137</v>
       </c>
       <c r="D208" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="E208">
         <v>2</v>
@@ -22747,7 +22744,7 @@
         <v>92.317596566523605</v>
       </c>
       <c r="I208" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J208" s="24">
         <f>AVERAGE(3.91,4.07)</f>
@@ -22764,7 +22761,7 @@
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B209" t="s">
         <v>139</v>
@@ -22791,7 +22788,7 @@
         <v>7.6824034334763951</v>
       </c>
       <c r="I209" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J209" s="24">
         <f>AVERAGE(27.05,27.53)</f>
@@ -22808,7 +22805,7 @@
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B210" t="s">
         <v>139</v>
@@ -22823,7 +22820,7 @@
         <v>3</v>
       </c>
       <c r="I210" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J210" s="24">
         <f>AVERAGE(3.69,3.81)</f>
@@ -22840,7 +22837,7 @@
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B211" t="s">
         <v>139</v>
@@ -22855,7 +22852,7 @@
         <v>3</v>
       </c>
       <c r="I211" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J211" s="24">
         <f>AVERAGE(2.42,2.42)</f>
@@ -22996,7 +22993,7 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B216" t="s">
         <v>139</v>
@@ -23018,12 +23015,12 @@
         <v>3.4589800000000004</v>
       </c>
       <c r="M216" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B217" t="s">
         <v>139</v>
@@ -23059,12 +23056,12 @@
         <v>2.9761099999999998</v>
       </c>
       <c r="M217" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B218" t="s">
         <v>139</v>
@@ -23100,12 +23097,12 @@
         <v>2.5168000000000004</v>
       </c>
       <c r="M218" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B219" t="s">
         <v>139</v>
@@ -23127,12 +23124,12 @@
         <v>3.89025</v>
       </c>
       <c r="M219" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B220" t="s">
         <v>139</v>
@@ -23168,12 +23165,12 @@
         <v>3.91906</v>
       </c>
       <c r="M220" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B221" t="s">
         <v>139</v>
@@ -23209,12 +23206,12 @@
         <v>2.6795999999999998</v>
       </c>
       <c r="M221" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B222" t="s">
         <v>139</v>
@@ -23236,12 +23233,12 @@
         <v>2.28552</v>
       </c>
       <c r="M222" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B223" t="s">
         <v>139</v>
@@ -23277,12 +23274,12 @@
         <v>2.2776000000000001</v>
       </c>
       <c r="M223" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B224" t="s">
         <v>139</v>
@@ -23318,12 +23315,12 @@
         <v>1.9539199999999999</v>
       </c>
       <c r="M224" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B225" t="s">
         <v>139</v>
@@ -23345,12 +23342,12 @@
         <v>2.7507999999999999</v>
       </c>
       <c r="M225" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B226" t="s">
         <v>139</v>
@@ -23386,12 +23383,12 @@
         <v>2.7477499999999999</v>
       </c>
       <c r="M226" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B227" t="s">
         <v>139</v>
@@ -23427,12 +23424,12 @@
         <v>1.8914400000000002</v>
       </c>
       <c r="M227" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B228" t="s">
         <v>139</v>
@@ -23454,12 +23451,12 @@
         <v>2.9165399999999999</v>
       </c>
       <c r="M228" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B229" t="s">
         <v>139</v>
@@ -23495,12 +23492,12 @@
         <v>2.9608799999999995</v>
       </c>
       <c r="M229" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B230" t="s">
         <v>139</v>
@@ -23536,12 +23533,12 @@
         <v>2.4230999999999998</v>
       </c>
       <c r="M230" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="231" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B231" t="s">
         <v>139</v>
@@ -23563,12 +23560,12 @@
         <v>2.1029100000000001</v>
       </c>
       <c r="M231" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B232" t="s">
         <v>139</v>
@@ -23604,12 +23601,12 @@
         <v>2.1321300000000001</v>
       </c>
       <c r="M232" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B233" t="s">
         <v>139</v>
@@ -23645,12 +23642,12 @@
         <v>1.9197599999999999</v>
       </c>
       <c r="M233" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="234" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B234" t="s">
         <v>139</v>
@@ -23672,12 +23669,12 @@
         <v>1.45791</v>
       </c>
       <c r="M234" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B235" t="s">
         <v>139</v>
@@ -23713,12 +23710,12 @@
         <v>1.3854600000000001</v>
       </c>
       <c r="M235" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B236" t="s">
         <v>139</v>
@@ -23754,12 +23751,12 @@
         <v>1.3926500000000002</v>
       </c>
       <c r="M236" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B237" t="s">
         <v>139</v>
@@ -23781,12 +23778,12 @@
         <v>4.5609200000000003</v>
       </c>
       <c r="M237" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B238" t="s">
         <v>139</v>
@@ -23822,12 +23819,12 @@
         <v>3.8614000000000006</v>
       </c>
       <c r="M238" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B239" t="s">
         <v>139</v>
@@ -23863,12 +23860,12 @@
         <v>3.1916000000000002</v>
       </c>
       <c r="M239" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B240" t="s">
         <v>139</v>
@@ -23890,12 +23887,12 @@
         <v>2.1723899999999996</v>
       </c>
       <c r="M240" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B241" t="s">
         <v>139</v>
@@ -23931,12 +23928,12 @@
         <v>2.2550400000000002</v>
       </c>
       <c r="M241" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B242" t="s">
         <v>139</v>
@@ -23972,12 +23969,12 @@
         <v>1.9466999999999999</v>
       </c>
       <c r="M242" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B243" t="s">
         <v>139</v>
@@ -23999,12 +23996,12 @@
         <v>3.0811499999999996</v>
       </c>
       <c r="M243" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B244" t="s">
         <v>139</v>
@@ -24040,12 +24037,12 @@
         <v>3.0192800000000002</v>
       </c>
       <c r="M244" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B245" t="s">
         <v>139</v>
@@ -24081,12 +24078,12 @@
         <v>2.5615000000000006</v>
       </c>
       <c r="M245" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B246" t="s">
         <v>139</v>
@@ -24108,12 +24105,12 @@
         <v>2.02217</v>
       </c>
       <c r="M246" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="247" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B247" t="s">
         <v>139</v>
@@ -24149,12 +24146,12 @@
         <v>1.9288800000000004</v>
       </c>
       <c r="M247" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B248" t="s">
         <v>139</v>
@@ -24190,12 +24187,12 @@
         <v>1.5435999999999999</v>
       </c>
       <c r="M248" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B249" t="s">
         <v>139</v>
@@ -24215,7 +24212,7 @@
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B250" t="s">
         <v>139</v>
@@ -24237,7 +24234,7 @@
         <v>90.156486622917711</v>
       </c>
       <c r="I250" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J250">
         <v>3.29</v>
@@ -24245,7 +24242,7 @@
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B251" t="s">
         <v>139</v>
@@ -24267,7 +24264,7 @@
         <v>9.8435133770822887</v>
       </c>
       <c r="I251" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J251">
         <v>23.1</v>
@@ -24286,6 +24283,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000AF577DD6E8D684CAFF1362865632EC1" ma:contentTypeVersion="14" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="124ec2e8304c3c5bf89d682421b875f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2f148fa0-8849-43ca-a1ad-3219566f6285" xmlns:ns4="3b7cc9eb-1f2c-44c2-aef1-68ff51cd8f88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="464bcc6cf6fa934ceccd475991ae2ccb" ns3:_="" ns4:_="">
     <xsd:import namespace="2f148fa0-8849-43ca-a1ad-3219566f6285"/>
@@ -24514,36 +24526,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A662E54A-967B-44BB-90F9-1599E728B1A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DF2204-8892-4A94-90A5-6DCDBF4AC498}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2f148fa0-8849-43ca-a1ad-3219566f6285"/>
-    <ds:schemaRef ds:uri="3b7cc9eb-1f2c-44c2-aef1-68ff51cd8f88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24566,9 +24552,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DF2204-8892-4A94-90A5-6DCDBF4AC498}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A662E54A-967B-44BB-90F9-1599E728B1A7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2f148fa0-8849-43ca-a1ad-3219566f6285"/>
+    <ds:schemaRef ds:uri="3b7cc9eb-1f2c-44c2-aef1-68ff51cd8f88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>